<commit_message>
Update For Shear Design
Update for Shear design
</commit_message>
<xml_diff>
--- a/AE Sakib/Narail/2021_22/Bridges/Kalishankar Pur Khal Footoverbridge/Girder Reiforcement Calcualtion/T_Giredr_Data.xlsx
+++ b/AE Sakib/Narail/2021_22/Bridges/Kalishankar Pur Khal Footoverbridge/Girder Reiforcement Calcualtion/T_Giredr_Data.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +809,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>